<commit_message>
Added correlation scatters and correlation matrix for all variables. Handled outliers, based on leverage, standarized errors and DFFITS. Estimated models for both cases without handling outliers and handling them by removing some observations.
</commit_message>
<xml_diff>
--- a/data/dane_zuzycie_energii.xlsx
+++ b/data/dane_zuzycie_energii.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SGGW-przedmioty\semestr 3\Ekonometria\dane\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B747C86-96F0-4242-92E1-7B7442F63444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Powiat</t>
   </si>
@@ -41,7 +47,7 @@
     <t>X2 - ludność na 1 km2 [os/km2]</t>
   </si>
   <si>
-    <t>X3 - mieszkania oddane do użytkowania na 1000 ludności [liczba budynków]</t>
+    <t>X3 - mieszkania oddane do użytkowania na 1000 ludności [-]</t>
   </si>
   <si>
     <t>X4 - przeciętne miesięczne wynagrodzenie brutto [zł]</t>
@@ -50,13 +56,16 @@
     <t>X5 - stopa bezrobocia rejestrowanego [%]</t>
   </si>
   <si>
-    <t>X6 - ludność w wieku 10-29 [os]</t>
-  </si>
-  <si>
-    <t>X7 - liczba obiektów  noclegówych [ob.]</t>
-  </si>
-  <si>
-    <t>X8 - wskaźnik urbanizacji [%]</t>
+    <t>X6 - ludność w wieku 15-34 [os]</t>
+  </si>
+  <si>
+    <t>X7 - liczba mieszkań [-]</t>
+  </si>
+  <si>
+    <t>X8 - powierzchnia użytkowa mieszkań [m2]</t>
+  </si>
+  <si>
+    <t>X9 - wskaźnik urbanizacji [%]</t>
   </si>
   <si>
     <t>Powiat białobrzeski</t>
@@ -188,16 +197,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.#0"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.#0"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +213,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
@@ -215,6 +221,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
@@ -222,355 +229,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -578,319 +249,33 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1148,33 +533,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="17.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="12.7777777777778" customWidth="1"/>
-    <col min="4" max="4" width="15.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="18.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="15.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="10.2222222222222" customWidth="1"/>
-    <col min="8" max="8" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="10.8888888888889" customWidth="1"/>
-    <col min="10" max="10" width="12.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="72" spans="1:10">
+    <row r="1" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1205,13 +590,16 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
-        <v>752.05</v>
+        <v>707.6</v>
       </c>
       <c r="C2" s="4">
         <v>2.72</v>
@@ -1229,21 +617,24 @@
         <v>10.1</v>
       </c>
       <c r="H2" s="6">
-        <v>9028</v>
+        <v>9725</v>
       </c>
       <c r="I2" s="7">
-        <v>5</v>
-      </c>
-      <c r="J2">
+        <v>11833</v>
+      </c>
+      <c r="J2" s="7">
+        <v>973610</v>
+      </c>
+      <c r="K2">
         <v>23.6</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
-        <v>639.31</v>
+        <v>708.5</v>
       </c>
       <c r="C3" s="4">
         <v>2.5</v>
@@ -1261,21 +652,24 @@
         <v>13.1</v>
       </c>
       <c r="H3" s="6">
-        <v>22173</v>
+        <v>24902</v>
       </c>
       <c r="I3" s="7">
-        <v>11</v>
-      </c>
-      <c r="J3">
+        <v>31131</v>
+      </c>
+      <c r="J3" s="7">
+        <v>2357060</v>
+      </c>
+      <c r="K3">
         <v>52.6</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>769.93</v>
+        <v>721.6</v>
       </c>
       <c r="C4" s="4">
         <v>2.82</v>
@@ -1293,21 +687,24 @@
         <v>11.3</v>
       </c>
       <c r="H4" s="6">
-        <v>29125</v>
+        <v>31822</v>
       </c>
       <c r="I4" s="7">
-        <v>12</v>
-      </c>
-      <c r="J4">
+        <v>34836</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3231888</v>
+      </c>
+      <c r="K4">
         <v>28.3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
-        <v>630.91</v>
+        <v>694</v>
       </c>
       <c r="C5" s="4">
         <v>2.58</v>
@@ -1325,21 +722,24 @@
         <v>18.5</v>
       </c>
       <c r="H5" s="6">
-        <v>10784</v>
+        <v>12186</v>
       </c>
       <c r="I5" s="7">
-        <v>2</v>
-      </c>
-      <c r="J5">
+        <v>16198</v>
+      </c>
+      <c r="J5" s="7">
+        <v>1140062</v>
+      </c>
+      <c r="K5">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
-        <v>995.22</v>
+        <v>1077.8</v>
       </c>
       <c r="C6" s="4">
         <v>2.46</v>
@@ -1354,27 +754,30 @@
         <v>4352.3</v>
       </c>
       <c r="G6" s="5">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H6" s="6">
-        <v>20188</v>
+        <v>22364</v>
       </c>
       <c r="I6" s="7">
-        <v>11</v>
-      </c>
-      <c r="J6">
+        <v>35319</v>
+      </c>
+      <c r="J6" s="7">
+        <v>3560595</v>
+      </c>
+      <c r="K6">
         <v>55.4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
-        <v>959.41</v>
+        <v>968.2</v>
       </c>
       <c r="C7" s="4">
-        <v>2.49</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="D7" s="5">
         <v>77.7</v>
@@ -1389,30 +792,33 @@
         <v>3.3</v>
       </c>
       <c r="H7" s="6">
-        <v>23036</v>
+        <v>25605</v>
       </c>
       <c r="I7" s="7">
-        <v>11</v>
-      </c>
-      <c r="J7">
+        <v>36565</v>
+      </c>
+      <c r="J7" s="7">
+        <v>3239850</v>
+      </c>
+      <c r="K7">
         <v>35.1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
-        <v>638.91</v>
+        <v>729.4</v>
       </c>
       <c r="C8" s="4">
         <v>2.54</v>
       </c>
       <c r="D8" s="5">
-        <v>66.6</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="E8" s="5">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F8" s="4">
         <v>4930.22</v>
@@ -1421,21 +827,24 @@
         <v>12.8</v>
       </c>
       <c r="H8" s="6">
-        <v>14978</v>
+        <v>16801</v>
       </c>
       <c r="I8" s="7">
-        <v>9</v>
-      </c>
-      <c r="J8">
+        <v>22088</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1884398</v>
+      </c>
+      <c r="K8">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3">
-        <v>799.12</v>
+        <v>979.4</v>
       </c>
       <c r="C9" s="4">
         <v>2.38</v>
@@ -1453,21 +862,24 @@
         <v>10.9</v>
       </c>
       <c r="H9" s="6">
-        <v>24599</v>
+        <v>27406</v>
       </c>
       <c r="I9" s="7">
-        <v>23</v>
-      </c>
-      <c r="J9">
+        <v>44131</v>
+      </c>
+      <c r="J9" s="7">
+        <v>4513662</v>
+      </c>
+      <c r="K9">
         <v>51.1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3">
-        <v>1152.47</v>
+        <v>633.6</v>
       </c>
       <c r="C10" s="4">
         <v>2.52</v>
@@ -1476,7 +888,7 @@
         <v>47.1</v>
       </c>
       <c r="E10" s="5">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F10" s="4">
         <v>3567.68</v>
@@ -1485,27 +897,30 @@
         <v>12.6</v>
       </c>
       <c r="H10" s="6">
-        <v>8259</v>
+        <v>9296</v>
       </c>
       <c r="I10" s="7">
-        <v>2</v>
-      </c>
-      <c r="J10">
+        <v>13264</v>
+      </c>
+      <c r="J10" s="7">
+        <v>1091815</v>
+      </c>
+      <c r="K10">
         <v>16.3</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3">
-        <v>714.37</v>
+        <v>833</v>
       </c>
       <c r="C11" s="4">
-        <v>2.47</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D11" s="5">
-        <v>40.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="E11" s="5">
         <v>1.6</v>
@@ -1514,24 +929,27 @@
         <v>3369.26</v>
       </c>
       <c r="G11" s="5">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H11" s="6">
-        <v>7986</v>
+        <v>8854</v>
       </c>
       <c r="I11" s="7">
-        <v>12</v>
-      </c>
-      <c r="J11">
+        <v>11507</v>
+      </c>
+      <c r="J11" s="7">
+        <v>967572</v>
+      </c>
+      <c r="K11">
         <v>22.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
-        <v>857.69</v>
+        <v>840.4</v>
       </c>
       <c r="C12" s="4">
         <v>2.67</v>
@@ -1540,36 +958,39 @@
         <v>43</v>
       </c>
       <c r="E12" s="5">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F12" s="4">
         <v>3359.63</v>
       </c>
       <c r="G12" s="5">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="H12" s="6">
-        <v>11780</v>
+        <v>12821</v>
       </c>
       <c r="I12" s="7">
-        <v>3</v>
-      </c>
-      <c r="J12">
+        <v>15167</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1267752</v>
+      </c>
+      <c r="K12">
         <v>27.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3">
-        <v>881.94</v>
+        <v>904</v>
       </c>
       <c r="C13" s="4">
-        <v>2.53</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="D13" s="5">
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="E13" s="5">
         <v>4.2</v>
@@ -1581,21 +1002,24 @@
         <v>6.8</v>
       </c>
       <c r="H13" s="6">
-        <v>36014</v>
+        <v>40540</v>
       </c>
       <c r="I13" s="7">
-        <v>13</v>
-      </c>
-      <c r="J13">
+        <v>55224</v>
+      </c>
+      <c r="J13" s="7">
+        <v>4883606</v>
+      </c>
+      <c r="K13">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3">
-        <v>680.36</v>
+        <v>689</v>
       </c>
       <c r="C14" s="4">
         <v>2.5</v>
@@ -1610,24 +1034,27 @@
         <v>3262.68</v>
       </c>
       <c r="G14" s="5">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H14" s="6">
-        <v>19001</v>
+        <v>21168</v>
       </c>
       <c r="I14" s="7">
-        <v>3</v>
-      </c>
-      <c r="J14">
+        <v>25091</v>
+      </c>
+      <c r="J14" s="7">
+        <v>2073150</v>
+      </c>
+      <c r="K14">
         <v>42.3</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3">
-        <v>818.03</v>
+        <v>852.7</v>
       </c>
       <c r="C15" s="4">
         <v>2.36</v>
@@ -1642,24 +1069,27 @@
         <v>4790.57</v>
       </c>
       <c r="G15" s="5">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H15" s="6">
-        <v>18230</v>
+        <v>21071</v>
       </c>
       <c r="I15" s="7">
-        <v>14</v>
-      </c>
-      <c r="J15">
+        <v>29774</v>
+      </c>
+      <c r="J15" s="7">
+        <v>2662861</v>
+      </c>
+      <c r="K15">
         <v>49.9</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3">
-        <v>713.49</v>
+        <v>821.4</v>
       </c>
       <c r="C16" s="4">
         <v>3.37</v>
@@ -1677,21 +1107,24 @@
         <v>14.2</v>
       </c>
       <c r="H16" s="6">
-        <v>25168</v>
+        <v>26973</v>
       </c>
       <c r="I16" s="7">
-        <v>5</v>
-      </c>
-      <c r="J16">
+        <v>24549</v>
+      </c>
+      <c r="J16" s="7">
+        <v>2472886</v>
+      </c>
+      <c r="K16">
         <v>3.8</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3">
-        <v>790.06</v>
+        <v>791.1</v>
       </c>
       <c r="C17" s="4">
         <v>2.69</v>
@@ -1709,24 +1142,27 @@
         <v>11.7</v>
       </c>
       <c r="H17" s="6">
-        <v>18816</v>
+        <v>20707</v>
       </c>
       <c r="I17" s="7">
-        <v>5</v>
-      </c>
-      <c r="J17">
+        <v>24607</v>
+      </c>
+      <c r="J17" s="7">
+        <v>1988427</v>
+      </c>
+      <c r="K17">
         <v>33.5</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="3">
-        <v>1036.33</v>
+        <v>1031.4000000000001</v>
       </c>
       <c r="C18" s="4">
-        <v>2.51</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D18" s="5">
         <v>200.4</v>
@@ -1741,21 +1177,24 @@
         <v>5.8</v>
       </c>
       <c r="H18" s="6">
-        <v>27423</v>
+        <v>30532</v>
       </c>
       <c r="I18" s="7">
-        <v>12</v>
-      </c>
-      <c r="J18">
+        <v>46733</v>
+      </c>
+      <c r="J18" s="7">
+        <v>4113950</v>
+      </c>
+      <c r="K18">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3">
-        <v>1104.38</v>
+        <v>1303</v>
       </c>
       <c r="C19" s="4">
         <v>2.27</v>
@@ -1773,21 +1212,24 @@
         <v>5.5</v>
       </c>
       <c r="H19" s="6">
-        <v>39417</v>
+        <v>42932</v>
       </c>
       <c r="I19" s="7">
-        <v>23</v>
-      </c>
-      <c r="J19">
+        <v>74375</v>
+      </c>
+      <c r="J19" s="7">
+        <v>9733282</v>
+      </c>
+      <c r="K19">
         <v>44.7</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3">
-        <v>739.58</v>
+        <v>786.6</v>
       </c>
       <c r="C20" s="4">
         <v>3</v>
@@ -1805,21 +1247,24 @@
         <v>15.1</v>
       </c>
       <c r="H20" s="6">
-        <v>28862</v>
+        <v>31309</v>
       </c>
       <c r="I20" s="7">
-        <v>16</v>
-      </c>
-      <c r="J20">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>34851</v>
+      </c>
+      <c r="J20" s="7">
+        <v>3279308</v>
+      </c>
+      <c r="K20">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3">
-        <v>665.17</v>
+        <v>770.1</v>
       </c>
       <c r="C21" s="4">
         <v>2.59</v>
@@ -1837,24 +1282,27 @@
         <v>12.6</v>
       </c>
       <c r="H21" s="6">
-        <v>21842</v>
+        <v>24138</v>
       </c>
       <c r="I21" s="7">
-        <v>10</v>
-      </c>
-      <c r="J21">
+        <v>30176</v>
+      </c>
+      <c r="J21" s="7">
+        <v>2385269</v>
+      </c>
+      <c r="K21">
         <v>30.4</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3">
-        <v>866.92</v>
+        <v>1027.5999999999999</v>
       </c>
       <c r="C22" s="4">
-        <v>2.26</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D22" s="5">
         <v>656.3</v>
@@ -1869,21 +1317,24 @@
         <v>5.3</v>
       </c>
       <c r="H22" s="6">
-        <v>33017</v>
+        <v>38174</v>
       </c>
       <c r="I22" s="7">
-        <v>21</v>
-      </c>
-      <c r="J22">
+        <v>61701</v>
+      </c>
+      <c r="J22" s="7">
+        <v>5982509</v>
+      </c>
+      <c r="K22">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3">
-        <v>836.58</v>
+        <v>833.5</v>
       </c>
       <c r="C23" s="4">
         <v>2.85</v>
@@ -1901,21 +1352,24 @@
         <v>12</v>
       </c>
       <c r="H23" s="6">
-        <v>13860</v>
+        <v>15065</v>
       </c>
       <c r="I23" s="7">
-        <v>5</v>
-      </c>
-      <c r="J23">
+        <v>16105</v>
+      </c>
+      <c r="J23" s="7">
+        <v>1373007</v>
+      </c>
+      <c r="K23">
         <v>38.4</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3">
-        <v>851.52</v>
+        <v>624.79999999999995</v>
       </c>
       <c r="C24" s="4">
         <v>2.66</v>
@@ -1933,21 +1387,24 @@
         <v>21.9</v>
       </c>
       <c r="H24" s="6">
-        <v>10999</v>
+        <v>12144</v>
       </c>
       <c r="I24" s="7">
-        <v>5</v>
-      </c>
-      <c r="J24">
+        <v>14726</v>
+      </c>
+      <c r="J24" s="7">
+        <v>1142051</v>
+      </c>
+      <c r="K24">
         <v>14.1</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3">
-        <v>670.8</v>
+        <v>754.8</v>
       </c>
       <c r="C25" s="4">
         <v>2.62</v>
@@ -1956,30 +1413,33 @@
         <v>62.5</v>
       </c>
       <c r="E25" s="5">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F25" s="4">
         <v>3399.46</v>
       </c>
       <c r="G25" s="5">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="H25" s="6">
-        <v>13266</v>
+        <v>14698</v>
       </c>
       <c r="I25" s="7">
-        <v>3</v>
-      </c>
-      <c r="J25">
+        <v>18387</v>
+      </c>
+      <c r="J25" s="7">
+        <v>1562114</v>
+      </c>
+      <c r="K25">
         <v>37.4</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="3">
-        <v>638.9</v>
+        <v>609.6</v>
       </c>
       <c r="C26" s="4">
         <v>3.08</v>
@@ -1997,21 +1457,24 @@
         <v>22</v>
       </c>
       <c r="H26" s="6">
-        <v>40706</v>
+        <v>44761</v>
       </c>
       <c r="I26" s="7">
-        <v>14</v>
-      </c>
-      <c r="J26">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>45557</v>
+      </c>
+      <c r="J26" s="7">
+        <v>3896569</v>
+      </c>
+      <c r="K26">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3">
-        <v>712.12</v>
+        <v>782.5</v>
       </c>
       <c r="C27" s="4">
         <v>2.92</v>
@@ -2029,21 +1492,24 @@
         <v>7.4</v>
       </c>
       <c r="H27" s="6">
-        <v>22196</v>
+        <v>23916</v>
       </c>
       <c r="I27" s="7">
-        <v>6</v>
-      </c>
-      <c r="J27">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>26198</v>
+      </c>
+      <c r="J27" s="7">
+        <v>2364577</v>
+      </c>
+      <c r="K27">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3">
-        <v>676.76</v>
+        <v>743</v>
       </c>
       <c r="C28" s="4">
         <v>2.74</v>
@@ -2052,30 +1518,33 @@
         <v>61.9</v>
       </c>
       <c r="E28" s="5">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F28" s="4">
         <v>3393.19</v>
       </c>
       <c r="G28" s="5">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="H28" s="6">
-        <v>13948</v>
+        <v>15140</v>
       </c>
       <c r="I28" s="7">
-        <v>5</v>
-      </c>
-      <c r="J28">
+        <v>16746</v>
+      </c>
+      <c r="J28" s="7">
+        <v>1275513</v>
+      </c>
+      <c r="K28">
         <v>34.5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="3">
-        <v>876.98</v>
+        <v>877.5</v>
       </c>
       <c r="C29" s="4">
         <v>2.68</v>
@@ -2093,21 +1562,24 @@
         <v>8.1</v>
       </c>
       <c r="H29" s="6">
-        <v>20169</v>
+        <v>22828</v>
       </c>
       <c r="I29" s="7">
-        <v>4</v>
-      </c>
-      <c r="J29">
+        <v>29318</v>
+      </c>
+      <c r="J29" s="7">
+        <v>2615545</v>
+      </c>
+      <c r="K29">
         <v>43.4</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="3">
-        <v>775.4</v>
+        <v>781.6</v>
       </c>
       <c r="C30" s="4">
         <v>2.41</v>
@@ -2125,21 +1597,24 @@
         <v>8</v>
       </c>
       <c r="H30" s="6">
-        <v>13420</v>
+        <v>14907</v>
       </c>
       <c r="I30" s="7">
-        <v>6</v>
-      </c>
-      <c r="J30">
-        <v>38.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>21017</v>
+      </c>
+      <c r="J30" s="7">
+        <v>1753785</v>
+      </c>
+      <c r="K30">
+        <v>38.299999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" s="3">
-        <v>862.55</v>
+        <v>552.6</v>
       </c>
       <c r="C31" s="4">
         <v>2.81</v>
@@ -2157,24 +1632,27 @@
         <v>28.5</v>
       </c>
       <c r="H31" s="6">
-        <v>10192</v>
+        <v>11487</v>
       </c>
       <c r="I31" s="7">
-        <v>8</v>
-      </c>
-      <c r="J31">
+        <v>13170</v>
+      </c>
+      <c r="J31" s="7">
+        <v>1032743</v>
+      </c>
+      <c r="K31">
         <v>29.7</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" s="3">
-        <v>1064.49</v>
+        <v>1157.5999999999999</v>
       </c>
       <c r="C32" s="4">
-        <v>2.53</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="D32" s="5">
         <v>213.7</v>
@@ -2183,27 +1661,30 @@
         <v>7.3</v>
       </c>
       <c r="F32" s="4">
-        <v>4800.81</v>
+        <v>4800.8100000000004</v>
       </c>
       <c r="G32" s="5">
         <v>3.1</v>
       </c>
       <c r="H32" s="6">
-        <v>25481</v>
+        <v>27683</v>
       </c>
       <c r="I32" s="7">
-        <v>19</v>
-      </c>
-      <c r="J32">
-        <v>35.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>43961</v>
+      </c>
+      <c r="J32" s="7">
+        <v>4849143</v>
+      </c>
+      <c r="K32">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="3">
-        <v>816.92</v>
+        <v>764.4</v>
       </c>
       <c r="C33" s="4">
         <v>2.48</v>
@@ -2218,24 +1699,27 @@
         <v>3396.09</v>
       </c>
       <c r="G33" s="5">
-        <v>9.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="H33" s="6">
-        <v>16826</v>
+        <v>18631</v>
       </c>
       <c r="I33" s="7">
-        <v>5</v>
-      </c>
-      <c r="J33">
+        <v>24498</v>
+      </c>
+      <c r="J33" s="7">
+        <v>1964965</v>
+      </c>
+      <c r="K33">
         <v>29.3</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="3">
-        <v>880.61</v>
+        <v>913.1</v>
       </c>
       <c r="C34" s="4">
         <v>2.64</v>
@@ -2253,21 +1737,24 @@
         <v>11.2</v>
       </c>
       <c r="H34" s="6">
-        <v>56237</v>
+        <v>63429</v>
       </c>
       <c r="I34" s="7">
-        <v>16</v>
-      </c>
-      <c r="J34">
+        <v>83204</v>
+      </c>
+      <c r="J34" s="7">
+        <v>8283450</v>
+      </c>
+      <c r="K34">
         <v>68.8</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="3">
-        <v>692.45</v>
+        <v>741</v>
       </c>
       <c r="C35" s="4">
         <v>2.83</v>
@@ -2285,21 +1772,24 @@
         <v>6.9</v>
       </c>
       <c r="H35" s="6">
-        <v>19111</v>
+        <v>21321</v>
       </c>
       <c r="I35" s="7">
-        <v>7</v>
-      </c>
-      <c r="J35">
+        <v>23180</v>
+      </c>
+      <c r="J35" s="7">
+        <v>1888466</v>
+      </c>
+      <c r="K35">
         <v>36.6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36" s="3">
-        <v>984.91</v>
+        <v>641</v>
       </c>
       <c r="C36" s="4">
         <v>2.84</v>
@@ -2317,21 +1807,24 @@
         <v>15.2</v>
       </c>
       <c r="H36" s="6">
-        <v>9493</v>
+        <v>10454</v>
       </c>
       <c r="I36" s="7">
-        <v>3</v>
-      </c>
-      <c r="J36">
+        <v>12243</v>
+      </c>
+      <c r="J36" s="7">
+        <v>995334</v>
+      </c>
+      <c r="K36">
         <v>21.6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="3">
-        <v>725.99</v>
+        <v>762.1</v>
       </c>
       <c r="C37" s="4">
         <v>2.87</v>
@@ -2349,24 +1842,27 @@
         <v>17.3</v>
       </c>
       <c r="H37" s="6">
-        <v>10353</v>
+        <v>11214</v>
       </c>
       <c r="I37" s="7">
-        <v>2</v>
-      </c>
-      <c r="J37">
+        <v>12111</v>
+      </c>
+      <c r="J37" s="7">
+        <v>1089651</v>
+      </c>
+      <c r="K37">
         <v>27.4</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="3">
-        <v>781.05</v>
+        <v>826.2</v>
       </c>
       <c r="C38" s="4">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D38" s="5">
         <v>143</v>
@@ -2381,24 +1877,27 @@
         <v>13</v>
       </c>
       <c r="H38" s="6">
-        <v>16828</v>
+        <v>19187</v>
       </c>
       <c r="I38" s="7">
-        <v>9</v>
-      </c>
-      <c r="J38">
+        <v>30649</v>
+      </c>
+      <c r="J38" s="7">
+        <v>1941013</v>
+      </c>
+      <c r="K38">
         <v>61.6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="3">
-        <v>602.93</v>
+        <v>544.20000000000005</v>
       </c>
       <c r="C39" s="4">
-        <v>2.32</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="D39" s="5">
         <v>1828</v>
@@ -2413,24 +1912,27 @@
         <v>12.5</v>
       </c>
       <c r="H39" s="6">
-        <v>11936</v>
+        <v>14129</v>
       </c>
       <c r="I39" s="7">
-        <v>3</v>
-      </c>
-      <c r="J39">
+        <v>19107</v>
+      </c>
+      <c r="J39" s="7">
+        <v>1210241</v>
+      </c>
+      <c r="K39">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B40" s="3">
-        <v>631.14</v>
+        <v>636.70000000000005</v>
       </c>
       <c r="C40" s="4">
-        <v>2.05</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="D40" s="5">
         <v>1377.7</v>
@@ -2445,21 +1947,24 @@
         <v>8.6</v>
       </c>
       <c r="H40" s="6">
-        <v>25326</v>
+        <v>29879</v>
       </c>
       <c r="I40" s="7">
-        <v>16</v>
-      </c>
-      <c r="J40">
+        <v>50768</v>
+      </c>
+      <c r="J40" s="7">
+        <v>3104573</v>
+      </c>
+      <c r="K40">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B41" s="3">
-        <v>669.85</v>
+        <v>623.70000000000005</v>
       </c>
       <c r="C41" s="4">
         <v>2.19</v>
@@ -2468,7 +1973,7 @@
         <v>1923.3</v>
       </c>
       <c r="E41" s="5">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F41" s="4">
         <v>3851.41</v>
@@ -2477,21 +1982,24 @@
         <v>15.9</v>
       </c>
       <c r="H41" s="6">
-        <v>47793</v>
+        <v>55665</v>
       </c>
       <c r="I41" s="7">
-        <v>13</v>
-      </c>
-      <c r="J41">
+        <v>83015</v>
+      </c>
+      <c r="J41" s="7">
+        <v>5363626</v>
+      </c>
+      <c r="K41">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B42" s="3">
-        <v>694.27</v>
+        <v>678.3</v>
       </c>
       <c r="C42" s="4">
         <v>2.09</v>
@@ -2509,21 +2017,24 @@
         <v>6.8</v>
       </c>
       <c r="H42" s="6">
-        <v>17125</v>
+        <v>20454</v>
       </c>
       <c r="I42" s="7">
-        <v>8</v>
-      </c>
-      <c r="J42">
+        <v>32225</v>
+      </c>
+      <c r="J42" s="7">
+        <v>2708556</v>
+      </c>
+      <c r="K42">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B43" s="3">
-        <v>1029.98</v>
+        <v>912.2</v>
       </c>
       <c r="C43" s="4">
         <v>1.73</v>
@@ -2541,17 +2052,271 @@
         <v>2.6</v>
       </c>
       <c r="H43" s="6">
-        <v>313330</v>
+        <v>411201</v>
       </c>
       <c r="I43" s="7">
-        <v>148</v>
-      </c>
-      <c r="J43">
+        <v>932574</v>
+      </c>
+      <c r="J43" s="7">
+        <v>83165992</v>
+      </c>
+      <c r="K43">
         <v>100</v>
       </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L44" s="7"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L46" s="7"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L47" s="7"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L48" s="7"/>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L49" s="7"/>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L50" s="7"/>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L51" s="7"/>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L52" s="7"/>
+    </row>
+    <row r="53" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L53" s="7"/>
+    </row>
+    <row r="54" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L54" s="7"/>
+    </row>
+    <row r="55" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L55" s="7"/>
+    </row>
+    <row r="56" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L56" s="7"/>
+    </row>
+    <row r="57" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L57" s="7"/>
+    </row>
+    <row r="58" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L58" s="7"/>
+    </row>
+    <row r="59" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L59" s="7"/>
+    </row>
+    <row r="60" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L60" s="7"/>
+    </row>
+    <row r="61" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L61" s="7"/>
+    </row>
+    <row r="62" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L62" s="7"/>
+    </row>
+    <row r="63" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L63" s="7"/>
+    </row>
+    <row r="64" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L64" s="7"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L65" s="7"/>
+    </row>
+    <row r="66" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L66" s="7"/>
+    </row>
+    <row r="67" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L67" s="7"/>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L68" s="7"/>
+    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L69" s="7"/>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L70" s="7"/>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L71" s="7"/>
+    </row>
+    <row r="72" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L72" s="7"/>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L73" s="7"/>
+    </row>
+    <row r="74" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L74" s="7"/>
+    </row>
+    <row r="75" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L75" s="7"/>
+    </row>
+    <row r="76" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L76" s="7"/>
+    </row>
+    <row r="77" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L77" s="7"/>
+    </row>
+    <row r="78" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L78" s="7"/>
+    </row>
+    <row r="79" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L79" s="7"/>
+    </row>
+    <row r="80" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L80" s="7"/>
+    </row>
+    <row r="81" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L81" s="7"/>
+    </row>
+    <row r="82" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L82" s="7"/>
+    </row>
+    <row r="83" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L83" s="7"/>
+    </row>
+    <row r="84" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L84" s="7"/>
+    </row>
+    <row r="85" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L85" s="7"/>
+    </row>
+    <row r="86" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L86" s="7"/>
+    </row>
+    <row r="87" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L87" s="7"/>
+    </row>
+    <row r="88" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L88" s="7"/>
+    </row>
+    <row r="89" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L89" s="7"/>
+    </row>
+    <row r="90" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L90" s="7"/>
+    </row>
+    <row r="91" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L91" s="7"/>
+    </row>
+    <row r="92" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L92" s="7"/>
+    </row>
+    <row r="93" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L93" s="7"/>
+    </row>
+    <row r="94" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L94" s="7"/>
+    </row>
+    <row r="95" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L95" s="7"/>
+    </row>
+    <row r="96" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L96" s="7"/>
+    </row>
+    <row r="97" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L97" s="7"/>
+    </row>
+    <row r="98" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L98" s="7"/>
+    </row>
+    <row r="99" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L99" s="7"/>
+    </row>
+    <row r="100" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L100" s="7"/>
+    </row>
+    <row r="101" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L101" s="7"/>
+    </row>
+    <row r="102" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L102" s="7"/>
+    </row>
+    <row r="103" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L103" s="7"/>
+    </row>
+    <row r="104" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L104" s="7"/>
+    </row>
+    <row r="105" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L105" s="7"/>
+    </row>
+    <row r="106" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L106" s="7"/>
+    </row>
+    <row r="107" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L107" s="7"/>
+    </row>
+    <row r="108" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L108" s="7"/>
+    </row>
+    <row r="109" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L109" s="7"/>
+    </row>
+    <row r="110" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L110" s="7"/>
+    </row>
+    <row r="111" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L111" s="7"/>
+    </row>
+    <row r="112" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L112" s="7"/>
+    </row>
+    <row r="113" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L113" s="7"/>
+    </row>
+    <row r="114" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L114" s="7"/>
+    </row>
+    <row r="115" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L115" s="7"/>
+    </row>
+    <row r="116" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L116" s="7"/>
+    </row>
+    <row r="117" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L117" s="7"/>
+    </row>
+    <row r="118" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L118" s="7"/>
+    </row>
+    <row r="119" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L119" s="7"/>
+    </row>
+    <row r="120" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L120" s="7"/>
+    </row>
+    <row r="121" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L121" s="7"/>
+    </row>
+    <row r="122" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L122" s="7"/>
+    </row>
+    <row r="123" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L123" s="7"/>
+    </row>
+    <row r="124" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L124" s="7"/>
+    </row>
+    <row r="125" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L125" s="7"/>
+    </row>
+    <row r="126" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L126" s="7"/>
+    </row>
+    <row r="127" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L127" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>